<commit_message>
Updated ITA model - 2025-07-29 10:10
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD2AB552-B6AA-4F55-A623-45F1C8CF74A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{537BCE17-3BFF-4461-B742-EC16C55EA10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{382320D9-2528-4CDA-B2FF-D55AFA8189D6}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{D6772C4F-6FE2-45E8-82E7-412DA7E6B9AD}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2589,7 +2589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C5F549-FC1D-49C0-9DA4-C25C752079A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2AE0558-3331-42BB-B59A-A99801962104}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5514,7 +5514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2806861A-E09F-48D3-9AF2-40C39C27A9BB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EA2FCD-25CB-4AD0-AE10-6758D52551C4}">
   <dimension ref="A2:T146"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13599,7 +13599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FEE1D36-CEC7-40E0-9A20-FEA250882020}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CE23CA-A344-41B8-9A35-4375263A34EA}">
   <dimension ref="A2:S348"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-29 13:49
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{537BCE17-3BFF-4461-B742-EC16C55EA10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF6A2629-EE03-4222-8B9E-AACD411704C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{D6772C4F-6FE2-45E8-82E7-412DA7E6B9AD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{B0751BE8-3C0D-47D6-9516-CE491B0E5E6F}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2589,7 +2589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2AE0558-3331-42BB-B59A-A99801962104}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BBBE48-49B4-4659-AE9A-4AFFCD67F2E0}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5514,7 +5514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EA2FCD-25CB-4AD0-AE10-6758D52551C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C6B5DF-A153-4132-A40C-B80803599987}">
   <dimension ref="A2:T146"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13599,7 +13599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CE23CA-A344-41B8-9A35-4375263A34EA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D21010-F7CE-4832-88C8-C79D30E39FB1}">
   <dimension ref="A2:S348"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 08:19
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0355FDB-33D9-4633-87CD-5FD8324F15D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{43273C37-1BC1-46B3-8457-3CD0ACA2501A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{48720D72-FB40-4221-AB7E-FB28AA1CC96B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{2EDC5C15-47B1-4E98-B381-985034838B15}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2589,7 +2589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E526DFD-DFAA-40DD-BC5F-6F596BEE2AAA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE1BA1D-C107-48B1-BFF0-B7A797D8021A}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5514,7 +5514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1047B517-A3F3-464D-AD9D-337329697A40}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9B0595-0263-432A-91EE-B3A0599C55F3}">
   <dimension ref="A2:T146"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13599,7 +13599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9591968A-4DA7-42B5-87A3-273F3661A34B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B224A4B-A21D-4BD0-AE7B-CE6C17F79B99}">
   <dimension ref="A2:S348"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 08:26
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43273C37-1BC1-46B3-8457-3CD0ACA2501A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FE1787D-75C9-4385-8DDE-71907094F85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{2EDC5C15-47B1-4E98-B381-985034838B15}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{F6B26415-7FF5-4E40-A58D-E2FEF394CD19}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2589,7 +2589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE1BA1D-C107-48B1-BFF0-B7A797D8021A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017A0ECC-D06C-46FD-8040-A4915F229B24}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5514,7 +5514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9B0595-0263-432A-91EE-B3A0599C55F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F04818A-FA3B-4408-AA5E-91DF48D55CD7}">
   <dimension ref="A2:T146"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13599,7 +13599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B224A4B-A21D-4BD0-AE7B-CE6C17F79B99}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E263B6CD-E938-474B-B06D-402FDBF31F43}">
   <dimension ref="A2:S348"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 08:34
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FE1787D-75C9-4385-8DDE-71907094F85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C591E73C-9010-4B83-B695-792BEDB5336B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{F6B26415-7FF5-4E40-A58D-E2FEF394CD19}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{3F0EBC1A-52CF-45B7-9389-308CEC5EDDC4}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2589,7 +2589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017A0ECC-D06C-46FD-8040-A4915F229B24}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6433530D-9C09-41C4-BF3F-4AC8179A4694}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5514,7 +5514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F04818A-FA3B-4408-AA5E-91DF48D55CD7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45858AC8-6399-41F7-9C88-B7C84796364E}">
   <dimension ref="A2:T146"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13599,7 +13599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E263B6CD-E938-474B-B06D-402FDBF31F43}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691E3EA4-419B-471A-8196-C2AFFA7D61A9}">
   <dimension ref="A2:S348"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 08:36
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C591E73C-9010-4B83-B695-792BEDB5336B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C966D943-F14F-4E4C-A15F-57C2678D6D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{3F0EBC1A-52CF-45B7-9389-308CEC5EDDC4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{C455E47F-385F-48EA-8BE7-3D1E4C5F9544}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4618" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4618" uniqueCount="728">
   <si>
     <t>process</t>
   </si>
@@ -1265,6 +1265,9 @@
   </si>
   <si>
     <t>San Filippo del Mela power station_1</t>
+  </si>
+  <si>
+    <t>annual</t>
   </si>
   <si>
     <t>Tuscania solar farm_--</t>
@@ -2589,7 +2592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6433530D-9C09-41C4-BF3F-4AC8179A4694}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA64188F-F0FF-46D1-A961-92F0C0DF0A4E}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -2598,10 +2601,10 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="J2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
@@ -2624,7 +2627,7 @@
         <v>2050</v>
       </c>
       <c r="G3" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="J3" t="s">
         <v>219</v>
@@ -2650,7 +2653,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -2674,7 +2677,7 @@
         <v>225</v>
       </c>
       <c r="K4" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="M4" t="s">
         <v>227</v>
@@ -2691,7 +2694,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -2709,13 +2712,13 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="G5" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="J5" t="s">
         <v>225</v>
       </c>
       <c r="K5" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="M5" t="s">
         <v>227</v>
@@ -2732,7 +2735,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -2756,7 +2759,7 @@
         <v>225</v>
       </c>
       <c r="K6" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="M6" t="s">
         <v>227</v>
@@ -2773,7 +2776,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -2797,7 +2800,7 @@
         <v>225</v>
       </c>
       <c r="K7" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="M7" t="s">
         <v>227</v>
@@ -2814,7 +2817,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -2832,13 +2835,13 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="J8" t="s">
         <v>225</v>
       </c>
       <c r="K8" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="M8" t="s">
         <v>227</v>
@@ -2855,7 +2858,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -2879,7 +2882,7 @@
         <v>225</v>
       </c>
       <c r="K9" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="M9" t="s">
         <v>227</v>
@@ -2896,7 +2899,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -2914,13 +2917,13 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="G10" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="J10" t="s">
         <v>225</v>
       </c>
       <c r="K10" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="M10" t="s">
         <v>227</v>
@@ -2937,7 +2940,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -2961,7 +2964,7 @@
         <v>225</v>
       </c>
       <c r="K11" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="M11" t="s">
         <v>227</v>
@@ -2978,7 +2981,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -3002,7 +3005,7 @@
         <v>225</v>
       </c>
       <c r="K12" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="M12" t="s">
         <v>227</v>
@@ -3019,7 +3022,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -3037,13 +3040,13 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="J13" t="s">
         <v>225</v>
       </c>
       <c r="K13" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="M13" t="s">
         <v>227</v>
@@ -3060,7 +3063,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -3084,7 +3087,7 @@
         <v>225</v>
       </c>
       <c r="K14" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="M14" t="s">
         <v>227</v>
@@ -3101,7 +3104,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -3119,13 +3122,13 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="G15" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="J15" t="s">
         <v>225</v>
       </c>
       <c r="K15" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="M15" t="s">
         <v>227</v>
@@ -3142,7 +3145,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -3166,7 +3169,7 @@
         <v>225</v>
       </c>
       <c r="K16" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="M16" t="s">
         <v>227</v>
@@ -3183,7 +3186,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -3207,7 +3210,7 @@
         <v>225</v>
       </c>
       <c r="K17" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="M17" t="s">
         <v>227</v>
@@ -3224,7 +3227,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -3242,13 +3245,13 @@
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="J18" t="s">
         <v>225</v>
       </c>
       <c r="K18" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="M18" t="s">
         <v>227</v>
@@ -3265,7 +3268,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
@@ -3289,7 +3292,7 @@
         <v>225</v>
       </c>
       <c r="K19" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="M19" t="s">
         <v>227</v>
@@ -3306,7 +3309,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -3324,13 +3327,13 @@
         <v>0.70000000000000007</v>
       </c>
       <c r="G20" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="J20" t="s">
         <v>225</v>
       </c>
       <c r="K20" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="M20" t="s">
         <v>227</v>
@@ -3347,7 +3350,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -3371,7 +3374,7 @@
         <v>225</v>
       </c>
       <c r="K21" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M21" t="s">
         <v>227</v>
@@ -3388,7 +3391,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -3412,7 +3415,7 @@
         <v>225</v>
       </c>
       <c r="K22" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="M22" t="s">
         <v>227</v>
@@ -3429,7 +3432,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
@@ -3447,13 +3450,13 @@
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="J23" t="s">
         <v>225</v>
       </c>
       <c r="K23" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="M23" t="s">
         <v>227</v>
@@ -3470,7 +3473,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -3494,7 +3497,7 @@
         <v>225</v>
       </c>
       <c r="K24" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="M24" t="s">
         <v>227</v>
@@ -3511,7 +3514,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
@@ -3535,7 +3538,7 @@
         <v>225</v>
       </c>
       <c r="K25" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="M25" t="s">
         <v>227</v>
@@ -3552,7 +3555,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -3576,7 +3579,7 @@
         <v>225</v>
       </c>
       <c r="K26" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="M26" t="s">
         <v>227</v>
@@ -3593,7 +3596,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -3617,7 +3620,7 @@
         <v>225</v>
       </c>
       <c r="K27" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="M27" t="s">
         <v>227</v>
@@ -3634,7 +3637,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B28" t="s">
         <v>25</v>
@@ -3658,7 +3661,7 @@
         <v>225</v>
       </c>
       <c r="K28" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="M28" t="s">
         <v>227</v>
@@ -3675,7 +3678,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
@@ -3699,7 +3702,7 @@
         <v>225</v>
       </c>
       <c r="K29" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="M29" t="s">
         <v>227</v>
@@ -3716,7 +3719,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B30" t="s">
         <v>25</v>
@@ -3739,7 +3742,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B31" t="s">
         <v>25</v>
@@ -3762,7 +3765,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
@@ -3785,7 +3788,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -3808,7 +3811,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B34" t="s">
         <v>14</v>
@@ -3831,7 +3834,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B35" t="s">
         <v>14</v>
@@ -3854,7 +3857,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B36" t="s">
         <v>208</v>
@@ -3877,7 +3880,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B37" t="s">
         <v>208</v>
@@ -3895,12 +3898,12 @@
         <v>0.42</v>
       </c>
       <c r="G37" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B38" t="s">
         <v>208</v>
@@ -3923,7 +3926,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B39" t="s">
         <v>208</v>
@@ -3946,7 +3949,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B40" t="s">
         <v>208</v>
@@ -3964,15 +3967,15 @@
         <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B41" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C41" t="s">
         <v>12</v>
@@ -3992,10 +3995,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B42" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C42" t="s">
         <v>12</v>
@@ -4015,10 +4018,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B43" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C43" t="s">
         <v>12</v>
@@ -4038,7 +4041,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B44" t="s">
         <v>25</v>
@@ -4061,7 +4064,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B45" t="s">
         <v>25</v>
@@ -4084,7 +4087,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B46" t="s">
         <v>25</v>
@@ -4107,7 +4110,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B47" t="s">
         <v>148</v>
@@ -4130,7 +4133,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B48" t="s">
         <v>148</v>
@@ -4148,12 +4151,12 @@
         <v>0.85000000000000009</v>
       </c>
       <c r="G48" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B49" t="s">
         <v>148</v>
@@ -4176,7 +4179,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B50" t="s">
         <v>148</v>
@@ -4199,7 +4202,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B51" t="s">
         <v>148</v>
@@ -4217,12 +4220,12 @@
         <v>4</v>
       </c>
       <c r="G51" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B52" t="s">
         <v>150</v>
@@ -4245,7 +4248,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B53" t="s">
         <v>150</v>
@@ -4263,12 +4266,12 @@
         <v>0.35000000000000003</v>
       </c>
       <c r="G53" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B54" t="s">
         <v>150</v>
@@ -4291,7 +4294,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B55" t="s">
         <v>150</v>
@@ -4314,7 +4317,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B56" t="s">
         <v>150</v>
@@ -4332,12 +4335,12 @@
         <v>4</v>
       </c>
       <c r="G56" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B57" t="s">
         <v>150</v>
@@ -4360,7 +4363,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B58" t="s">
         <v>150</v>
@@ -4378,12 +4381,12 @@
         <v>0.25</v>
       </c>
       <c r="G58" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B59" t="s">
         <v>150</v>
@@ -4406,7 +4409,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B60" t="s">
         <v>150</v>
@@ -4429,7 +4432,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B61" t="s">
         <v>150</v>
@@ -4447,12 +4450,12 @@
         <v>4</v>
       </c>
       <c r="G61" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B62" t="s">
         <v>25</v>
@@ -4475,7 +4478,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B63" t="s">
         <v>25</v>
@@ -4498,7 +4501,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B64" t="s">
         <v>25</v>
@@ -4521,7 +4524,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B65" t="s">
         <v>14</v>
@@ -4544,7 +4547,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B66" t="s">
         <v>14</v>
@@ -4567,7 +4570,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B67" t="s">
         <v>14</v>
@@ -4590,7 +4593,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B68" t="s">
         <v>150</v>
@@ -4613,7 +4616,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B69" t="s">
         <v>150</v>
@@ -4631,12 +4634,12 @@
         <v>0.25</v>
       </c>
       <c r="G69" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B70" t="s">
         <v>150</v>
@@ -4659,7 +4662,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B71" t="s">
         <v>150</v>
@@ -4682,7 +4685,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B72" t="s">
         <v>150</v>
@@ -4700,15 +4703,15 @@
         <v>4</v>
       </c>
       <c r="G72" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B73" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C73" t="s">
         <v>12</v>
@@ -4728,10 +4731,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B74" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C74" t="s">
         <v>12</v>
@@ -4751,10 +4754,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B75" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C75" t="s">
         <v>12</v>
@@ -4774,7 +4777,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B76" t="s">
         <v>14</v>
@@ -4797,7 +4800,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B77" t="s">
         <v>14</v>
@@ -4820,7 +4823,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B78" t="s">
         <v>14</v>
@@ -4843,7 +4846,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B79" t="s">
         <v>208</v>
@@ -4866,7 +4869,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B80" t="s">
         <v>208</v>
@@ -4884,12 +4887,12 @@
         <v>0.13</v>
       </c>
       <c r="G80" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B81" t="s">
         <v>208</v>
@@ -4912,7 +4915,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B82" t="s">
         <v>208</v>
@@ -4935,7 +4938,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B83" t="s">
         <v>208</v>
@@ -4953,12 +4956,12 @@
         <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B84" t="s">
         <v>208</v>
@@ -4981,7 +4984,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B85" t="s">
         <v>208</v>
@@ -4999,12 +5002,12 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G85" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B86" t="s">
         <v>208</v>
@@ -5027,7 +5030,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B87" t="s">
         <v>208</v>
@@ -5050,7 +5053,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B88" t="s">
         <v>208</v>
@@ -5068,12 +5071,12 @@
         <v>1.5</v>
       </c>
       <c r="G88" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B89" t="s">
         <v>14</v>
@@ -5096,7 +5099,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B90" t="s">
         <v>14</v>
@@ -5119,7 +5122,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B91" t="s">
         <v>14</v>
@@ -5142,7 +5145,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B92" t="s">
         <v>14</v>
@@ -5165,7 +5168,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B93" t="s">
         <v>14</v>
@@ -5188,7 +5191,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B94" t="s">
         <v>14</v>
@@ -5211,7 +5214,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B95" t="s">
         <v>14</v>
@@ -5234,7 +5237,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B96" t="s">
         <v>14</v>
@@ -5257,7 +5260,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B97" t="s">
         <v>14</v>
@@ -5280,7 +5283,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B98" t="s">
         <v>214</v>
@@ -5303,7 +5306,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B99" t="s">
         <v>214</v>
@@ -5321,12 +5324,12 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G99" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B100" t="s">
         <v>214</v>
@@ -5349,7 +5352,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B101" t="s">
         <v>214</v>
@@ -5372,7 +5375,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B102" t="s">
         <v>214</v>
@@ -5390,12 +5393,12 @@
         <v>3</v>
       </c>
       <c r="G102" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B103" t="s">
         <v>214</v>
@@ -5418,7 +5421,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B104" t="s">
         <v>214</v>
@@ -5436,12 +5439,12 @@
         <v>0.3</v>
       </c>
       <c r="G104" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B105" t="s">
         <v>214</v>
@@ -5464,7 +5467,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B106" t="s">
         <v>214</v>
@@ -5487,7 +5490,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B107" t="s">
         <v>214</v>
@@ -5505,7 +5508,7 @@
         <v>1.5</v>
       </c>
       <c r="G107" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>
@@ -5514,7 +5517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45858AC8-6399-41F7-9C88-B7C84796364E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27AAA46A-1384-4ED4-911C-79D635B559CF}">
   <dimension ref="A2:T146"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5523,10 +5526,10 @@
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="N2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.45">
@@ -5552,13 +5555,13 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="J3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="K3" t="s">
         <v>9</v>
@@ -5587,7 +5590,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -5623,10 +5626,10 @@
         <v>225</v>
       </c>
       <c r="O4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="P4" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="Q4" t="s">
         <v>227</v>
@@ -5643,7 +5646,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -5679,10 +5682,10 @@
         <v>225</v>
       </c>
       <c r="O5" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="P5" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="Q5" t="s">
         <v>227</v>
@@ -5699,7 +5702,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -5735,10 +5738,10 @@
         <v>225</v>
       </c>
       <c r="O6" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="P6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="Q6" t="s">
         <v>227</v>
@@ -5755,7 +5758,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -5791,10 +5794,10 @@
         <v>225</v>
       </c>
       <c r="O7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P7" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="Q7" t="s">
         <v>227</v>
@@ -5811,7 +5814,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -5847,10 +5850,10 @@
         <v>225</v>
       </c>
       <c r="O8" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="P8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="Q8" t="s">
         <v>227</v>
@@ -5867,7 +5870,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -5903,10 +5906,10 @@
         <v>225</v>
       </c>
       <c r="O9" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="P9" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="Q9" t="s">
         <v>227</v>
@@ -5923,7 +5926,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -5959,10 +5962,10 @@
         <v>225</v>
       </c>
       <c r="O10" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="P10" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="Q10" t="s">
         <v>227</v>
@@ -5979,7 +5982,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -6015,10 +6018,10 @@
         <v>225</v>
       </c>
       <c r="O11" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="P11" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="Q11" t="s">
         <v>227</v>
@@ -6035,7 +6038,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -6071,10 +6074,10 @@
         <v>225</v>
       </c>
       <c r="O12" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="P12" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="Q12" t="s">
         <v>227</v>
@@ -6091,7 +6094,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -6127,10 +6130,10 @@
         <v>225</v>
       </c>
       <c r="O13" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="P13" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="Q13" t="s">
         <v>227</v>
@@ -6147,7 +6150,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
@@ -6183,10 +6186,10 @@
         <v>225</v>
       </c>
       <c r="O14" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="P14" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="Q14" t="s">
         <v>227</v>
@@ -6203,7 +6206,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
@@ -6239,10 +6242,10 @@
         <v>225</v>
       </c>
       <c r="O15" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="P15" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="Q15" t="s">
         <v>227</v>
@@ -6259,7 +6262,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
@@ -6295,10 +6298,10 @@
         <v>225</v>
       </c>
       <c r="O16" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="P16" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="Q16" t="s">
         <v>227</v>
@@ -6315,7 +6318,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -6351,10 +6354,10 @@
         <v>225</v>
       </c>
       <c r="O17" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="P17" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="Q17" t="s">
         <v>227</v>
@@ -6371,7 +6374,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
@@ -6407,10 +6410,10 @@
         <v>225</v>
       </c>
       <c r="O18" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="P18" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="Q18" t="s">
         <v>227</v>
@@ -6427,7 +6430,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
@@ -6463,10 +6466,10 @@
         <v>225</v>
       </c>
       <c r="O19" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="P19" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="Q19" t="s">
         <v>227</v>
@@ -6483,7 +6486,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
@@ -6519,10 +6522,10 @@
         <v>225</v>
       </c>
       <c r="O20" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="P20" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="Q20" t="s">
         <v>227</v>
@@ -6539,7 +6542,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
@@ -6575,10 +6578,10 @@
         <v>225</v>
       </c>
       <c r="O21" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="P21" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="Q21" t="s">
         <v>227</v>
@@ -6595,7 +6598,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
@@ -6631,10 +6634,10 @@
         <v>225</v>
       </c>
       <c r="O22" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="P22" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="Q22" t="s">
         <v>227</v>
@@ -6651,7 +6654,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
@@ -6687,10 +6690,10 @@
         <v>225</v>
       </c>
       <c r="O23" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="P23" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="Q23" t="s">
         <v>227</v>
@@ -6707,7 +6710,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -6743,10 +6746,10 @@
         <v>225</v>
       </c>
       <c r="O24" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="P24" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="Q24" t="s">
         <v>227</v>
@@ -6763,7 +6766,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
@@ -6799,10 +6802,10 @@
         <v>225</v>
       </c>
       <c r="O25" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="P25" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="Q25" t="s">
         <v>227</v>
@@ -6819,7 +6822,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
@@ -6855,10 +6858,10 @@
         <v>225</v>
       </c>
       <c r="O26" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="P26" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="Q26" t="s">
         <v>227</v>
@@ -6875,7 +6878,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -6911,10 +6914,10 @@
         <v>225</v>
       </c>
       <c r="O27" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="P27" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="Q27" t="s">
         <v>227</v>
@@ -6931,7 +6934,7 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B28" t="s">
         <v>25</v>
@@ -6967,10 +6970,10 @@
         <v>225</v>
       </c>
       <c r="O28" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="P28" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="Q28" t="s">
         <v>227</v>
@@ -6987,7 +6990,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
@@ -7023,10 +7026,10 @@
         <v>225</v>
       </c>
       <c r="O29" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="P29" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="Q29" t="s">
         <v>227</v>
@@ -7043,7 +7046,7 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B30" t="s">
         <v>25</v>
@@ -7079,10 +7082,10 @@
         <v>225</v>
       </c>
       <c r="O30" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="P30" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="Q30" t="s">
         <v>227</v>
@@ -7099,7 +7102,7 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B31" t="s">
         <v>25</v>
@@ -7135,10 +7138,10 @@
         <v>225</v>
       </c>
       <c r="O31" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="P31" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="Q31" t="s">
         <v>227</v>
@@ -7155,7 +7158,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
@@ -7191,10 +7194,10 @@
         <v>225</v>
       </c>
       <c r="O32" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="P32" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Q32" t="s">
         <v>227</v>
@@ -7211,7 +7214,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
@@ -7247,10 +7250,10 @@
         <v>225</v>
       </c>
       <c r="O33" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="P33" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="Q33" t="s">
         <v>227</v>
@@ -7267,7 +7270,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B34" t="s">
         <v>25</v>
@@ -7303,10 +7306,10 @@
         <v>225</v>
       </c>
       <c r="O34" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="P34" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="Q34" t="s">
         <v>227</v>
@@ -7323,7 +7326,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B35" t="s">
         <v>25</v>
@@ -7359,10 +7362,10 @@
         <v>225</v>
       </c>
       <c r="O35" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="P35" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="Q35" t="s">
         <v>227</v>
@@ -7379,7 +7382,7 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B36" t="s">
         <v>25</v>
@@ -7415,10 +7418,10 @@
         <v>225</v>
       </c>
       <c r="O36" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="P36" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="Q36" t="s">
         <v>227</v>
@@ -7435,7 +7438,7 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B37" t="s">
         <v>25</v>
@@ -7471,10 +7474,10 @@
         <v>225</v>
       </c>
       <c r="O37" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="P37" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="Q37" t="s">
         <v>227</v>
@@ -7491,7 +7494,7 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B38" t="s">
         <v>25</v>
@@ -7527,10 +7530,10 @@
         <v>225</v>
       </c>
       <c r="O38" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="P38" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="Q38" t="s">
         <v>227</v>
@@ -7547,7 +7550,7 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B39" t="s">
         <v>25</v>
@@ -7583,10 +7586,10 @@
         <v>225</v>
       </c>
       <c r="O39" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="P39" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="Q39" t="s">
         <v>227</v>
@@ -7603,7 +7606,7 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B40" t="s">
         <v>25</v>
@@ -7639,10 +7642,10 @@
         <v>225</v>
       </c>
       <c r="O40" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="P40" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="Q40" t="s">
         <v>227</v>
@@ -7659,7 +7662,7 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B41" t="s">
         <v>25</v>
@@ -7695,10 +7698,10 @@
         <v>225</v>
       </c>
       <c r="O41" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="P41" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="Q41" t="s">
         <v>227</v>
@@ -7715,7 +7718,7 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B42" t="s">
         <v>25</v>
@@ -7751,10 +7754,10 @@
         <v>225</v>
       </c>
       <c r="O42" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="P42" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="Q42" t="s">
         <v>227</v>
@@ -7771,7 +7774,7 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B43" t="s">
         <v>25</v>
@@ -7807,10 +7810,10 @@
         <v>225</v>
       </c>
       <c r="O43" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="P43" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="Q43" t="s">
         <v>227</v>
@@ -7827,7 +7830,7 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B44" t="s">
         <v>25</v>
@@ -7863,10 +7866,10 @@
         <v>225</v>
       </c>
       <c r="O44" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="P44" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="Q44" t="s">
         <v>227</v>
@@ -7883,7 +7886,7 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B45" t="s">
         <v>25</v>
@@ -7919,10 +7922,10 @@
         <v>225</v>
       </c>
       <c r="O45" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="P45" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="Q45" t="s">
         <v>227</v>
@@ -7939,7 +7942,7 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B46" t="s">
         <v>25</v>
@@ -7975,10 +7978,10 @@
         <v>225</v>
       </c>
       <c r="O46" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="P46" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="Q46" t="s">
         <v>227</v>
@@ -7995,7 +7998,7 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B47" t="s">
         <v>25</v>
@@ -8031,10 +8034,10 @@
         <v>225</v>
       </c>
       <c r="O47" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="P47" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="Q47" t="s">
         <v>227</v>
@@ -8051,7 +8054,7 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B48" t="s">
         <v>25</v>
@@ -8087,10 +8090,10 @@
         <v>225</v>
       </c>
       <c r="O48" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="P48" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="Q48" t="s">
         <v>227</v>
@@ -8107,7 +8110,7 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B49" t="s">
         <v>25</v>
@@ -8143,10 +8146,10 @@
         <v>225</v>
       </c>
       <c r="O49" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="P49" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="Q49" t="s">
         <v>227</v>
@@ -8163,7 +8166,7 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B50" t="s">
         <v>25</v>
@@ -8199,10 +8202,10 @@
         <v>225</v>
       </c>
       <c r="O50" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="P50" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="Q50" t="s">
         <v>227</v>
@@ -8219,7 +8222,7 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B51" t="s">
         <v>25</v>
@@ -8255,10 +8258,10 @@
         <v>225</v>
       </c>
       <c r="O51" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="P51" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="Q51" t="s">
         <v>227</v>
@@ -8275,7 +8278,7 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B52" t="s">
         <v>25</v>
@@ -8311,10 +8314,10 @@
         <v>225</v>
       </c>
       <c r="O52" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="P52" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="Q52" t="s">
         <v>227</v>
@@ -8331,7 +8334,7 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B53" t="s">
         <v>25</v>
@@ -8367,10 +8370,10 @@
         <v>225</v>
       </c>
       <c r="O53" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="P53" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="Q53" t="s">
         <v>227</v>
@@ -8387,7 +8390,7 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B54" t="s">
         <v>25</v>
@@ -8423,10 +8426,10 @@
         <v>225</v>
       </c>
       <c r="O54" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="P54" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="Q54" t="s">
         <v>227</v>
@@ -8443,7 +8446,7 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B55" t="s">
         <v>25</v>
@@ -8479,10 +8482,10 @@
         <v>225</v>
       </c>
       <c r="O55" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="P55" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Q55" t="s">
         <v>227</v>
@@ -8499,7 +8502,7 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B56" t="s">
         <v>25</v>
@@ -8535,10 +8538,10 @@
         <v>225</v>
       </c>
       <c r="O56" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="P56" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="Q56" t="s">
         <v>227</v>
@@ -8555,7 +8558,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B57" t="s">
         <v>25</v>
@@ -8591,10 +8594,10 @@
         <v>225</v>
       </c>
       <c r="O57" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="P57" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="Q57" t="s">
         <v>227</v>
@@ -8611,7 +8614,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B58" t="s">
         <v>25</v>
@@ -8647,10 +8650,10 @@
         <v>225</v>
       </c>
       <c r="O58" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="P58" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="Q58" t="s">
         <v>227</v>
@@ -8667,7 +8670,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B59" t="s">
         <v>25</v>
@@ -8703,10 +8706,10 @@
         <v>225</v>
       </c>
       <c r="O59" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="P59" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="Q59" t="s">
         <v>227</v>
@@ -8723,7 +8726,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B60" t="s">
         <v>25</v>
@@ -8759,10 +8762,10 @@
         <v>225</v>
       </c>
       <c r="O60" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="P60" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="Q60" t="s">
         <v>227</v>
@@ -8779,7 +8782,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B61" t="s">
         <v>25</v>
@@ -8815,10 +8818,10 @@
         <v>225</v>
       </c>
       <c r="O61" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="P61" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="Q61" t="s">
         <v>227</v>
@@ -8835,7 +8838,7 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B62" t="s">
         <v>25</v>
@@ -8871,10 +8874,10 @@
         <v>225</v>
       </c>
       <c r="O62" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="P62" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="Q62" t="s">
         <v>227</v>
@@ -8891,7 +8894,7 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B63" t="s">
         <v>25</v>
@@ -8927,10 +8930,10 @@
         <v>225</v>
       </c>
       <c r="O63" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="P63" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="Q63" t="s">
         <v>227</v>
@@ -8947,7 +8950,7 @@
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B64" t="s">
         <v>25</v>
@@ -8983,10 +8986,10 @@
         <v>225</v>
       </c>
       <c r="O64" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="P64" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="Q64" t="s">
         <v>227</v>
@@ -9003,7 +9006,7 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B65" t="s">
         <v>25</v>
@@ -9039,10 +9042,10 @@
         <v>225</v>
       </c>
       <c r="O65" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="P65" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="Q65" t="s">
         <v>227</v>
@@ -9059,7 +9062,7 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B66" t="s">
         <v>25</v>
@@ -9095,10 +9098,10 @@
         <v>225</v>
       </c>
       <c r="O66" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="P66" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="Q66" t="s">
         <v>227</v>
@@ -9115,7 +9118,7 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B67" t="s">
         <v>25</v>
@@ -9151,10 +9154,10 @@
         <v>225</v>
       </c>
       <c r="O67" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="P67" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="Q67" t="s">
         <v>227</v>
@@ -9171,7 +9174,7 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B68" t="s">
         <v>25</v>
@@ -9207,10 +9210,10 @@
         <v>225</v>
       </c>
       <c r="O68" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="P68" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="Q68" t="s">
         <v>227</v>
@@ -9227,7 +9230,7 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B69" t="s">
         <v>25</v>
@@ -9263,10 +9266,10 @@
         <v>225</v>
       </c>
       <c r="O69" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="P69" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="Q69" t="s">
         <v>227</v>
@@ -9283,7 +9286,7 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B70" t="s">
         <v>25</v>
@@ -9319,10 +9322,10 @@
         <v>225</v>
       </c>
       <c r="O70" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="P70" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="Q70" t="s">
         <v>227</v>
@@ -9339,7 +9342,7 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B71" t="s">
         <v>25</v>
@@ -9375,10 +9378,10 @@
         <v>225</v>
       </c>
       <c r="O71" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="P71" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="Q71" t="s">
         <v>227</v>
@@ -9395,7 +9398,7 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B72" t="s">
         <v>25</v>
@@ -9431,10 +9434,10 @@
         <v>225</v>
       </c>
       <c r="O72" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="P72" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="Q72" t="s">
         <v>227</v>
@@ -9451,7 +9454,7 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B73" t="s">
         <v>25</v>
@@ -9487,10 +9490,10 @@
         <v>225</v>
       </c>
       <c r="O73" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="P73" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="Q73" t="s">
         <v>227</v>
@@ -9507,7 +9510,7 @@
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B74" t="s">
         <v>25</v>
@@ -9543,10 +9546,10 @@
         <v>225</v>
       </c>
       <c r="O74" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="P74" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="Q74" t="s">
         <v>227</v>
@@ -9563,7 +9566,7 @@
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B75" t="s">
         <v>25</v>
@@ -9599,10 +9602,10 @@
         <v>225</v>
       </c>
       <c r="O75" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="P75" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="Q75" t="s">
         <v>227</v>
@@ -9619,7 +9622,7 @@
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B76" t="s">
         <v>25</v>
@@ -9655,10 +9658,10 @@
         <v>225</v>
       </c>
       <c r="O76" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="P76" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="Q76" t="s">
         <v>227</v>
@@ -9675,7 +9678,7 @@
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B77" t="s">
         <v>25</v>
@@ -9711,10 +9714,10 @@
         <v>225</v>
       </c>
       <c r="O77" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="P77" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="Q77" t="s">
         <v>227</v>
@@ -9731,7 +9734,7 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B78" t="s">
         <v>25</v>
@@ -9767,10 +9770,10 @@
         <v>225</v>
       </c>
       <c r="O78" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="P78" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="Q78" t="s">
         <v>227</v>
@@ -9787,7 +9790,7 @@
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B79" t="s">
         <v>25</v>
@@ -9823,10 +9826,10 @@
         <v>225</v>
       </c>
       <c r="O79" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="P79" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="Q79" t="s">
         <v>227</v>
@@ -9843,7 +9846,7 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B80" t="s">
         <v>25</v>
@@ -9879,10 +9882,10 @@
         <v>225</v>
       </c>
       <c r="O80" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="P80" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="Q80" t="s">
         <v>227</v>
@@ -9899,7 +9902,7 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B81" t="s">
         <v>25</v>
@@ -9935,10 +9938,10 @@
         <v>225</v>
       </c>
       <c r="O81" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="P81" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="Q81" t="s">
         <v>227</v>
@@ -9955,7 +9958,7 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B82" t="s">
         <v>25</v>
@@ -9991,10 +9994,10 @@
         <v>225</v>
       </c>
       <c r="O82" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="P82" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="Q82" t="s">
         <v>227</v>
@@ -10011,7 +10014,7 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B83" t="s">
         <v>25</v>
@@ -10047,10 +10050,10 @@
         <v>225</v>
       </c>
       <c r="O83" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="P83" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="Q83" t="s">
         <v>227</v>
@@ -10067,7 +10070,7 @@
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B84" t="s">
         <v>25</v>
@@ -10103,10 +10106,10 @@
         <v>225</v>
       </c>
       <c r="O84" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="P84" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="Q84" t="s">
         <v>227</v>
@@ -10123,7 +10126,7 @@
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B85" t="s">
         <v>25</v>
@@ -10159,10 +10162,10 @@
         <v>225</v>
       </c>
       <c r="O85" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="P85" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="Q85" t="s">
         <v>227</v>
@@ -10179,7 +10182,7 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B86" t="s">
         <v>25</v>
@@ -10215,10 +10218,10 @@
         <v>225</v>
       </c>
       <c r="O86" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="P86" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="Q86" t="s">
         <v>227</v>
@@ -10235,7 +10238,7 @@
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B87" t="s">
         <v>25</v>
@@ -10271,10 +10274,10 @@
         <v>225</v>
       </c>
       <c r="O87" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="P87" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="Q87" t="s">
         <v>227</v>
@@ -10291,7 +10294,7 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B88" t="s">
         <v>25</v>
@@ -10327,10 +10330,10 @@
         <v>225</v>
       </c>
       <c r="O88" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="P88" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="Q88" t="s">
         <v>227</v>
@@ -10347,7 +10350,7 @@
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B89" t="s">
         <v>25</v>
@@ -10383,10 +10386,10 @@
         <v>225</v>
       </c>
       <c r="O89" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="P89" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="Q89" t="s">
         <v>227</v>
@@ -10403,7 +10406,7 @@
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B90" t="s">
         <v>25</v>
@@ -10439,10 +10442,10 @@
         <v>225</v>
       </c>
       <c r="O90" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="P90" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="Q90" t="s">
         <v>227</v>
@@ -10459,7 +10462,7 @@
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B91" t="s">
         <v>25</v>
@@ -10495,10 +10498,10 @@
         <v>225</v>
       </c>
       <c r="O91" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="P91" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="Q91" t="s">
         <v>227</v>
@@ -10515,7 +10518,7 @@
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B92" t="s">
         <v>25</v>
@@ -10551,10 +10554,10 @@
         <v>225</v>
       </c>
       <c r="O92" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="P92" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="Q92" t="s">
         <v>227</v>
@@ -10571,7 +10574,7 @@
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B93" t="s">
         <v>25</v>
@@ -10607,10 +10610,10 @@
         <v>225</v>
       </c>
       <c r="O93" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="P93" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="Q93" t="s">
         <v>227</v>
@@ -10627,7 +10630,7 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B94" t="s">
         <v>25</v>
@@ -10663,10 +10666,10 @@
         <v>225</v>
       </c>
       <c r="O94" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="P94" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="Q94" t="s">
         <v>227</v>
@@ -10683,7 +10686,7 @@
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B95" t="s">
         <v>25</v>
@@ -10719,10 +10722,10 @@
         <v>225</v>
       </c>
       <c r="O95" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="P95" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="Q95" t="s">
         <v>227</v>
@@ -10739,7 +10742,7 @@
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B96" t="s">
         <v>25</v>
@@ -10775,10 +10778,10 @@
         <v>225</v>
       </c>
       <c r="O96" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="P96" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="Q96" t="s">
         <v>227</v>
@@ -10795,7 +10798,7 @@
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B97" t="s">
         <v>25</v>
@@ -10831,10 +10834,10 @@
         <v>225</v>
       </c>
       <c r="O97" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="P97" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="Q97" t="s">
         <v>227</v>
@@ -10851,7 +10854,7 @@
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B98" t="s">
         <v>25</v>
@@ -10887,10 +10890,10 @@
         <v>225</v>
       </c>
       <c r="O98" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="P98" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="Q98" t="s">
         <v>227</v>
@@ -10907,7 +10910,7 @@
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B99" t="s">
         <v>25</v>
@@ -10943,10 +10946,10 @@
         <v>225</v>
       </c>
       <c r="O99" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="P99" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="Q99" t="s">
         <v>227</v>
@@ -10963,7 +10966,7 @@
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B100" t="s">
         <v>25</v>
@@ -10999,10 +11002,10 @@
         <v>225</v>
       </c>
       <c r="O100" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="P100" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="Q100" t="s">
         <v>227</v>
@@ -11019,7 +11022,7 @@
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B101" t="s">
         <v>25</v>
@@ -11055,10 +11058,10 @@
         <v>225</v>
       </c>
       <c r="O101" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="P101" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="Q101" t="s">
         <v>227</v>
@@ -11075,7 +11078,7 @@
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B102" t="s">
         <v>25</v>
@@ -11111,10 +11114,10 @@
         <v>225</v>
       </c>
       <c r="O102" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="P102" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="Q102" t="s">
         <v>227</v>
@@ -11131,7 +11134,7 @@
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B103" t="s">
         <v>25</v>
@@ -11167,10 +11170,10 @@
         <v>225</v>
       </c>
       <c r="O103" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="P103" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="Q103" t="s">
         <v>227</v>
@@ -11187,7 +11190,7 @@
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B104" t="s">
         <v>25</v>
@@ -11223,10 +11226,10 @@
         <v>225</v>
       </c>
       <c r="O104" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="P104" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="Q104" t="s">
         <v>227</v>
@@ -11243,7 +11246,7 @@
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B105" t="s">
         <v>25</v>
@@ -11279,10 +11282,10 @@
         <v>225</v>
       </c>
       <c r="O105" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="P105" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="Q105" t="s">
         <v>227</v>
@@ -11299,7 +11302,7 @@
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B106" t="s">
         <v>25</v>
@@ -11335,10 +11338,10 @@
         <v>225</v>
       </c>
       <c r="O106" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="P106" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="Q106" t="s">
         <v>227</v>
@@ -11355,7 +11358,7 @@
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B107" t="s">
         <v>25</v>
@@ -11391,10 +11394,10 @@
         <v>225</v>
       </c>
       <c r="O107" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="P107" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="Q107" t="s">
         <v>227</v>
@@ -11411,7 +11414,7 @@
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B108" t="s">
         <v>25</v>
@@ -11447,10 +11450,10 @@
         <v>225</v>
       </c>
       <c r="O108" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="P108" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="Q108" t="s">
         <v>227</v>
@@ -11467,7 +11470,7 @@
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B109" t="s">
         <v>25</v>
@@ -11503,10 +11506,10 @@
         <v>225</v>
       </c>
       <c r="O109" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P109" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="Q109" t="s">
         <v>227</v>
@@ -11523,7 +11526,7 @@
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B110" t="s">
         <v>25</v>
@@ -11559,10 +11562,10 @@
         <v>225</v>
       </c>
       <c r="O110" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="P110" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="Q110" t="s">
         <v>227</v>
@@ -11579,7 +11582,7 @@
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B111" t="s">
         <v>25</v>
@@ -11615,10 +11618,10 @@
         <v>225</v>
       </c>
       <c r="O111" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="P111" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="Q111" t="s">
         <v>227</v>
@@ -11635,7 +11638,7 @@
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B112" t="s">
         <v>25</v>
@@ -11671,10 +11674,10 @@
         <v>225</v>
       </c>
       <c r="O112" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="P112" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="Q112" t="s">
         <v>227</v>
@@ -11691,7 +11694,7 @@
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B113" t="s">
         <v>25</v>
@@ -11727,10 +11730,10 @@
         <v>225</v>
       </c>
       <c r="O113" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="P113" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="Q113" t="s">
         <v>227</v>
@@ -11747,7 +11750,7 @@
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B114" t="s">
         <v>25</v>
@@ -11783,10 +11786,10 @@
         <v>225</v>
       </c>
       <c r="O114" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="P114" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="Q114" t="s">
         <v>227</v>
@@ -11803,7 +11806,7 @@
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B115" t="s">
         <v>25</v>
@@ -11839,10 +11842,10 @@
         <v>225</v>
       </c>
       <c r="O115" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="P115" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Q115" t="s">
         <v>227</v>
@@ -11859,7 +11862,7 @@
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B116" t="s">
         <v>25</v>
@@ -11895,10 +11898,10 @@
         <v>225</v>
       </c>
       <c r="O116" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="P116" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="Q116" t="s">
         <v>227</v>
@@ -11915,7 +11918,7 @@
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B117" t="s">
         <v>25</v>
@@ -11951,10 +11954,10 @@
         <v>225</v>
       </c>
       <c r="O117" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="P117" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="Q117" t="s">
         <v>227</v>
@@ -11971,7 +11974,7 @@
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B118" t="s">
         <v>25</v>
@@ -12007,10 +12010,10 @@
         <v>225</v>
       </c>
       <c r="O118" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="P118" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="Q118" t="s">
         <v>227</v>
@@ -12027,7 +12030,7 @@
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B119" t="s">
         <v>25</v>
@@ -12063,10 +12066,10 @@
         <v>225</v>
       </c>
       <c r="O119" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="P119" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="Q119" t="s">
         <v>227</v>
@@ -12083,7 +12086,7 @@
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B120" t="s">
         <v>25</v>
@@ -12119,10 +12122,10 @@
         <v>225</v>
       </c>
       <c r="O120" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="P120" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Q120" t="s">
         <v>227</v>
@@ -12139,7 +12142,7 @@
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B121" t="s">
         <v>25</v>
@@ -12175,10 +12178,10 @@
         <v>225</v>
       </c>
       <c r="O121" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="P121" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="Q121" t="s">
         <v>227</v>
@@ -12195,7 +12198,7 @@
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B122" t="s">
         <v>25</v>
@@ -12231,10 +12234,10 @@
         <v>225</v>
       </c>
       <c r="O122" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="P122" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="Q122" t="s">
         <v>227</v>
@@ -12251,7 +12254,7 @@
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B123" t="s">
         <v>25</v>
@@ -12287,10 +12290,10 @@
         <v>225</v>
       </c>
       <c r="O123" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="P123" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="Q123" t="s">
         <v>227</v>
@@ -12307,7 +12310,7 @@
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B124" t="s">
         <v>25</v>
@@ -12343,10 +12346,10 @@
         <v>225</v>
       </c>
       <c r="O124" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="P124" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="Q124" t="s">
         <v>227</v>
@@ -12363,7 +12366,7 @@
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B125" t="s">
         <v>25</v>
@@ -12399,10 +12402,10 @@
         <v>225</v>
       </c>
       <c r="O125" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="P125" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="Q125" t="s">
         <v>227</v>
@@ -12419,7 +12422,7 @@
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B126" t="s">
         <v>25</v>
@@ -12455,10 +12458,10 @@
         <v>225</v>
       </c>
       <c r="O126" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="P126" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="Q126" t="s">
         <v>227</v>
@@ -12475,7 +12478,7 @@
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B127" t="s">
         <v>25</v>
@@ -12511,10 +12514,10 @@
         <v>225</v>
       </c>
       <c r="O127" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="P127" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="Q127" t="s">
         <v>227</v>
@@ -12531,7 +12534,7 @@
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B128" t="s">
         <v>25</v>
@@ -12567,10 +12570,10 @@
         <v>225</v>
       </c>
       <c r="O128" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="P128" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Q128" t="s">
         <v>227</v>
@@ -12587,7 +12590,7 @@
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B129" t="s">
         <v>25</v>
@@ -12623,10 +12626,10 @@
         <v>225</v>
       </c>
       <c r="O129" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="P129" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="Q129" t="s">
         <v>227</v>
@@ -12643,7 +12646,7 @@
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B130" t="s">
         <v>25</v>
@@ -12679,10 +12682,10 @@
         <v>225</v>
       </c>
       <c r="O130" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="P130" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Q130" t="s">
         <v>227</v>
@@ -12699,7 +12702,7 @@
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B131" t="s">
         <v>25</v>
@@ -12735,10 +12738,10 @@
         <v>225</v>
       </c>
       <c r="O131" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="P131" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="Q131" t="s">
         <v>227</v>
@@ -12755,7 +12758,7 @@
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B132" t="s">
         <v>25</v>
@@ -12791,10 +12794,10 @@
         <v>225</v>
       </c>
       <c r="O132" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="P132" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="Q132" t="s">
         <v>227</v>
@@ -12811,7 +12814,7 @@
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B133" t="s">
         <v>25</v>
@@ -12847,10 +12850,10 @@
         <v>225</v>
       </c>
       <c r="O133" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="P133" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="Q133" t="s">
         <v>227</v>
@@ -12867,7 +12870,7 @@
     </row>
     <row r="134" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B134" t="s">
         <v>25</v>
@@ -12903,10 +12906,10 @@
         <v>225</v>
       </c>
       <c r="O134" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="P134" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Q134" t="s">
         <v>227</v>
@@ -12923,7 +12926,7 @@
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B135" t="s">
         <v>25</v>
@@ -12959,10 +12962,10 @@
         <v>225</v>
       </c>
       <c r="O135" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="P135" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Q135" t="s">
         <v>227</v>
@@ -12979,7 +12982,7 @@
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B136" t="s">
         <v>196</v>
@@ -13015,10 +13018,10 @@
         <v>225</v>
       </c>
       <c r="O136" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="P136" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Q136" t="s">
         <v>227</v>
@@ -13035,7 +13038,7 @@
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B137" t="s">
         <v>196</v>
@@ -13071,10 +13074,10 @@
         <v>225</v>
       </c>
       <c r="O137" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="P137" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Q137" t="s">
         <v>227</v>
@@ -13091,7 +13094,7 @@
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B138" t="s">
         <v>196</v>
@@ -13127,10 +13130,10 @@
         <v>225</v>
       </c>
       <c r="O138" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="P138" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Q138" t="s">
         <v>227</v>
@@ -13147,7 +13150,7 @@
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B139" t="s">
         <v>196</v>
@@ -13183,10 +13186,10 @@
         <v>225</v>
       </c>
       <c r="O139" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="P139" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="Q139" t="s">
         <v>227</v>
@@ -13203,7 +13206,7 @@
     </row>
     <row r="140" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B140" t="s">
         <v>196</v>
@@ -13239,10 +13242,10 @@
         <v>225</v>
       </c>
       <c r="O140" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="P140" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="Q140" t="s">
         <v>227</v>
@@ -13259,7 +13262,7 @@
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B141" t="s">
         <v>196</v>
@@ -13295,10 +13298,10 @@
         <v>225</v>
       </c>
       <c r="O141" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="P141" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="Q141" t="s">
         <v>227</v>
@@ -13315,7 +13318,7 @@
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B142" t="s">
         <v>196</v>
@@ -13351,10 +13354,10 @@
         <v>225</v>
       </c>
       <c r="O142" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="P142" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="Q142" t="s">
         <v>227</v>
@@ -13371,7 +13374,7 @@
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B143" t="s">
         <v>196</v>
@@ -13407,10 +13410,10 @@
         <v>225</v>
       </c>
       <c r="O143" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="P143" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="Q143" t="s">
         <v>227</v>
@@ -13427,7 +13430,7 @@
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B144" t="s">
         <v>196</v>
@@ -13463,10 +13466,10 @@
         <v>225</v>
       </c>
       <c r="O144" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="P144" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="Q144" t="s">
         <v>227</v>
@@ -13483,7 +13486,7 @@
     </row>
     <row r="145" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B145" t="s">
         <v>196</v>
@@ -13519,10 +13522,10 @@
         <v>225</v>
       </c>
       <c r="O145" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="P145" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="Q145" t="s">
         <v>227</v>
@@ -13539,7 +13542,7 @@
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B146" t="s">
         <v>196</v>
@@ -13575,10 +13578,10 @@
         <v>225</v>
       </c>
       <c r="O146" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="P146" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Q146" t="s">
         <v>227</v>
@@ -13599,7 +13602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691E3EA4-419B-471A-8196-C2AFFA7D61A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE0A166-1270-4453-AB64-B73B1FB75E26}">
   <dimension ref="A2:S348"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13608,10 +13611,10 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.45">
@@ -23784,7 +23787,7 @@
         <v>228</v>
       </c>
       <c r="R194" t="s">
-        <v>229</v>
+        <v>409</v>
       </c>
       <c r="S194" t="s">
         <v>230</v>
@@ -23837,7 +23840,7 @@
         <v>228</v>
       </c>
       <c r="R195" t="s">
-        <v>229</v>
+        <v>409</v>
       </c>
       <c r="S195" t="s">
         <v>230</v>
@@ -23881,16 +23884,16 @@
         <v>211</v>
       </c>
       <c r="O196" t="s">
+        <v>410</v>
+      </c>
+      <c r="P196" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q196" t="s">
+        <v>228</v>
+      </c>
+      <c r="R196" t="s">
         <v>409</v>
-      </c>
-      <c r="P196" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q196" t="s">
-        <v>228</v>
-      </c>
-      <c r="R196" t="s">
-        <v>229</v>
       </c>
       <c r="S196" t="s">
         <v>232</v>
@@ -23934,7 +23937,7 @@
         <v>212</v>
       </c>
       <c r="O197" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="P197" t="s">
         <v>227</v>
@@ -23943,7 +23946,7 @@
         <v>228</v>
       </c>
       <c r="R197" t="s">
-        <v>229</v>
+        <v>409</v>
       </c>
       <c r="S197" t="s">
         <v>232</v>
@@ -23996,7 +23999,7 @@
         <v>228</v>
       </c>
       <c r="R198" t="s">
-        <v>229</v>
+        <v>409</v>
       </c>
       <c r="S198" t="s">
         <v>230</v>
@@ -24049,7 +24052,7 @@
         <v>228</v>
       </c>
       <c r="R199" t="s">
-        <v>229</v>
+        <v>409</v>
       </c>
       <c r="S199" t="s">
         <v>230</v>
@@ -24093,7 +24096,7 @@
         <v>217</v>
       </c>
       <c r="O200" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="P200" t="s">
         <v>227</v>
@@ -24102,7 +24105,7 @@
         <v>228</v>
       </c>
       <c r="R200" t="s">
-        <v>229</v>
+        <v>409</v>
       </c>
       <c r="S200" t="s">
         <v>232</v>
@@ -24146,7 +24149,7 @@
         <v>218</v>
       </c>
       <c r="O201" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="P201" t="s">
         <v>227</v>
@@ -24155,7 +24158,7 @@
         <v>228</v>
       </c>
       <c r="R201" t="s">
-        <v>229</v>
+        <v>409</v>
       </c>
       <c r="S201" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
Updated ITA model - 2025-07-30 16:48
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3355B5B4-02BB-44A0-B96F-0C8E8480AB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{280DD4AA-CEE4-4BF8-A674-A7BCACD86372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{78C4D191-E2E0-4973-A30D-12D588419712}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{9311FDA2-6B02-4150-ACF1-BB5DE899E46E}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2592,7 +2592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE0161F-1A69-4A61-BB68-4252D314FB17}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B934ACB1-C847-4751-BF0A-0C4E570B9432}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5517,7 +5517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39EF1BD9-547C-4D5B-85A2-5398D3AC0801}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51DA60A2-C71A-4579-BAAA-A7FF9D648E29}">
   <dimension ref="A2:T146"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13602,7 +13602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B8A42C-C591-4AA1-BDAF-FB057068CA9A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900E7074-802B-4CE7-A5EC-5EF272EF72E8}">
   <dimension ref="A2:S348"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-05 00:04
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7330B884-5EDB-439A-8BAA-3C81FB6A9D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F75F21C-F675-4255-A0FF-960F8B7C59D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{E30C7283-6013-4278-A493-C4AE9224547C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{B0C27A02-4B1F-4A61-9A1F-01DF89EB36E2}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2643,7 +2643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35CD990-95A7-4155-92E4-A8051415DBEA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C3EEFD-F871-40DC-ABA4-8CEBA70DB41A}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5568,7 +5568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B050357B-A1B8-4BE7-9139-E4A33C9D7E79}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1B163B-0235-479B-A789-4947C5FD3CA3}">
   <dimension ref="A2:T148"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13765,7 +13765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFC6C5E-1507-41F9-A44E-DA2C785BC1BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258DEC42-A28C-42FF-B9B4-A821DAA28D6A}">
   <dimension ref="A2:S350"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-05 00:09
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F75F21C-F675-4255-A0FF-960F8B7C59D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DA38582-DBDE-4D45-A5F5-C6AD9A1EA874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{B0C27A02-4B1F-4A61-9A1F-01DF89EB36E2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{B8F7286F-FC28-443D-AA8B-C98E6BC48504}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2643,7 +2643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C3EEFD-F871-40DC-ABA4-8CEBA70DB41A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF6D149-2AD7-4302-A26F-60C022C5FEEA}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5568,7 +5568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1B163B-0235-479B-A789-4947C5FD3CA3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FCE5EF6-6013-4483-BCC4-74EFF27BE15A}">
   <dimension ref="A2:T148"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13765,7 +13765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258DEC42-A28C-42FF-B9B4-A821DAA28D6A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB2D0BF-4539-478B-856A-A7A2009FA46E}">
   <dimension ref="A2:S350"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-05 00:14
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DA38582-DBDE-4D45-A5F5-C6AD9A1EA874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE0FB417-3DA3-4C3E-BA76-A1DEBC310176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{B8F7286F-FC28-443D-AA8B-C98E6BC48504}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{0A6C4C4D-FD96-4B04-81B0-083F07542CFC}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2643,7 +2643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF6D149-2AD7-4302-A26F-60C022C5FEEA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DAA53B-0D64-4832-992B-2D740ED885E3}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5568,7 +5568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FCE5EF6-6013-4483-BCC4-74EFF27BE15A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50480B5-B2D7-4441-A9F5-7FD44873371B}">
   <dimension ref="A2:T148"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13765,7 +13765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB2D0BF-4539-478B-856A-A7A2009FA46E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FEE0EDF-37CF-4B00-9FAE-8902D3C16724}">
   <dimension ref="A2:S350"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-05 00:25
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE0FB417-3DA3-4C3E-BA76-A1DEBC310176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA3D22CA-FF10-4582-BD3B-034710184917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{0A6C4C4D-FD96-4B04-81B0-083F07542CFC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{915A5A56-7E52-41E4-AB91-9C04D4CB918A}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2643,7 +2643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DAA53B-0D64-4832-992B-2D740ED885E3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C56B48D-65ED-4FE7-8CDD-0E6D4BD0FB43}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5568,7 +5568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50480B5-B2D7-4441-A9F5-7FD44873371B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202BB695-3F06-445E-983E-40090722D088}">
   <dimension ref="A2:T148"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13765,7 +13765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FEE0EDF-37CF-4B00-9FAE-8902D3C16724}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338DD435-CDB8-49BB-B9E8-5BDD42FFB075}">
   <dimension ref="A2:S350"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-05 01:01
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
+++ b/VerveStacks_ITA/vt_vervestacks_ITA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96236B7C-47D8-4CAC-B472-58B425694E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D11020D-F699-4C4D-81D0-C10B6A3D9952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{0451BD9F-BCE4-4703-9B0B-505E5C1DFAAC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{DF1BE1DF-87A5-44C6-8ED8-97BC2E1796C0}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -2643,7 +2643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15CF51F0-E53C-4168-BA72-86B5E37E79C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7DE4CA-09AB-4709-A18C-34EAF38D8775}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5568,7 +5568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E29224-C3E9-4F2A-94E0-CDD86791D399}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A1A524-98C3-4DFB-B5E9-5FA794FFACA7}">
   <dimension ref="A2:T148"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13765,7 +13765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1126EB0D-84FC-4685-9C41-C1F13C79BE84}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B681B882-4EFF-4D47-A6E0-B8E3C2350E2B}">
   <dimension ref="A2:S350"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>